<commit_message>
finish collecting raw data
</commit_message>
<xml_diff>
--- a/performance.xlsx
+++ b/performance.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B47585-AFC3-496F-B83D-B60F284368C5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D54E170-F6A5-495A-B282-3E5C7C7E4F6F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
   <si>
     <t>dog1</t>
   </si>
@@ -107,12 +107,6 @@
   </si>
   <si>
     <t xml:space="preserve">Full Model with fix-point </t>
-  </si>
-  <si>
-    <t>mAp</t>
-  </si>
-  <si>
-    <t>100%(2 classes)</t>
   </si>
 </sst>
 </file>
@@ -148,7 +142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -157,6 +151,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -450,8 +447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C4:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -484,7 +481,7 @@
       </c>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -501,7 +498,7 @@
       </c>
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C6" s="6"/>
+      <c r="C6" s="7"/>
       <c r="D6" s="1" t="s">
         <v>9</v>
       </c>
@@ -516,7 +513,7 @@
       </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C7" s="6"/>
+      <c r="C7" s="7"/>
       <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
@@ -531,7 +528,7 @@
       </c>
     </row>
     <row r="8" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C8" s="6"/>
+      <c r="C8" s="7"/>
       <c r="D8" s="1" t="s">
         <v>11</v>
       </c>
@@ -546,7 +543,7 @@
       </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C9" s="6"/>
+      <c r="C9" s="7"/>
       <c r="D9" s="1" t="s">
         <v>12</v>
       </c>
@@ -561,7 +558,7 @@
       </c>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C10" s="6"/>
+      <c r="C10" s="7"/>
       <c r="D10" s="1" t="s">
         <v>10</v>
       </c>
@@ -576,7 +573,7 @@
       </c>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C11" s="6"/>
+      <c r="C11" s="7"/>
       <c r="D11" s="1" t="s">
         <v>13</v>
       </c>
@@ -591,7 +588,7 @@
       </c>
     </row>
     <row r="12" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -608,7 +605,7 @@
       </c>
     </row>
     <row r="13" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C13" s="6"/>
+      <c r="C13" s="7"/>
       <c r="D13" s="1" t="s">
         <v>13</v>
       </c>
@@ -623,7 +620,7 @@
       </c>
     </row>
     <row r="14" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -640,7 +637,7 @@
       </c>
     </row>
     <row r="15" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C15" s="6"/>
+      <c r="C15" s="7"/>
       <c r="D15" s="1" t="s">
         <v>13</v>
       </c>
@@ -655,7 +652,7 @@
       </c>
     </row>
     <row r="16" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -672,7 +669,7 @@
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C17" s="6"/>
+      <c r="C17" s="7"/>
       <c r="D17" s="1" t="s">
         <v>13</v>
       </c>
@@ -699,6 +696,9 @@
       <c r="F18" s="3">
         <v>1</v>
       </c>
+      <c r="G18" s="3">
+        <v>0.99</v>
+      </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D19" s="1" t="s">
@@ -710,6 +710,9 @@
       <c r="F19" s="3">
         <v>0.62</v>
       </c>
+      <c r="G19" s="3">
+        <v>0.52</v>
+      </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D20" s="1" t="s">
@@ -721,6 +724,9 @@
       <c r="F20" s="3">
         <v>0.96</v>
       </c>
+      <c r="G20" s="3">
+        <v>0.96</v>
+      </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D21" s="1" t="s">
@@ -732,30 +738,39 @@
       <c r="F21" s="1">
         <v>46.367212000000002</v>
       </c>
-    </row>
-    <row r="22" spans="3:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D22" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>30</v>
+      <c r="G21" s="6">
+        <v>46.227164000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0.31</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0.88</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0.84</v>
       </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C23" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="D23" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E23" s="3">
-        <v>0.31</v>
+        <v>0.71</v>
       </c>
       <c r="F23" s="3">
-        <v>0.88</v>
+        <v>0.99</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0.99</v>
       </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.3">
@@ -763,10 +778,13 @@
         <v>18</v>
       </c>
       <c r="E24" s="3">
-        <v>0.71</v>
+        <v>0.54</v>
       </c>
       <c r="F24" s="3">
-        <v>0.99</v>
+        <v>0.96</v>
+      </c>
+      <c r="G24" s="3">
+        <v>0.97</v>
       </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.3">
@@ -774,10 +792,13 @@
         <v>18</v>
       </c>
       <c r="E25" s="3">
-        <v>0.54</v>
+        <v>0.32</v>
       </c>
       <c r="F25" s="3">
-        <v>0.96</v>
+        <v>0.99</v>
+      </c>
+      <c r="G25" s="3">
+        <v>0.98</v>
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.3">
@@ -785,184 +806,232 @@
         <v>18</v>
       </c>
       <c r="E26" s="3">
-        <v>0.32</v>
+        <v>0.68</v>
       </c>
       <c r="F26" s="3">
-        <v>0.99</v>
+        <v>0</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D27" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E27" s="3">
-        <v>0.68</v>
+        <v>0.39</v>
       </c>
       <c r="F27" s="3">
+        <v>0</v>
+      </c>
+      <c r="G27" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D28" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E28" s="3">
-        <v>0.39</v>
+        <v>0.7</v>
       </c>
       <c r="F28" s="3">
+        <v>0</v>
+      </c>
+      <c r="G28" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D29" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E29" s="3">
-        <v>0.7</v>
+        <v>0.51</v>
       </c>
       <c r="F29" s="3">
+        <v>0</v>
+      </c>
+      <c r="G29" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D30" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E30" s="3">
-        <v>0.51</v>
-      </c>
-      <c r="F30" s="3">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="E30" s="1">
+        <v>3.9323950000000001</v>
+      </c>
+      <c r="F30" s="1">
+        <v>49.033776000000003</v>
+      </c>
+      <c r="G30" s="6">
+        <v>46.235506999999998</v>
       </c>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C31" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D31" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E31" s="1">
-        <v>3.9323950000000001</v>
-      </c>
-      <c r="F31" s="1">
-        <v>49.033776000000003</v>
+        <v>8</v>
+      </c>
+      <c r="E31" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="F31" s="3">
+        <v>0.99</v>
+      </c>
+      <c r="G31" s="3">
+        <v>0.99</v>
       </c>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C32" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="D32" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E32" s="3">
-        <v>0.89</v>
+        <v>0.81</v>
       </c>
       <c r="F32" s="3">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="G32" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="F33" s="3">
+        <v>1</v>
+      </c>
+      <c r="G33" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="D34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E34" s="3">
+        <v>0</v>
+      </c>
+      <c r="F34" s="3">
+        <v>1</v>
+      </c>
+      <c r="G34" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="D35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" s="3">
+        <v>0.83</v>
+      </c>
+      <c r="F35" s="3">
+        <v>0</v>
+      </c>
+      <c r="G35" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="D36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" s="1">
+        <v>3.928356</v>
+      </c>
+      <c r="F36" s="1">
+        <v>51.211255000000001</v>
+      </c>
+      <c r="G36" s="6">
+        <v>46.131405000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C37" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="F37" s="3">
+        <v>1</v>
+      </c>
+      <c r="G37" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="D38" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E33" s="3">
-        <v>0.81</v>
-      </c>
-      <c r="F33" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D34" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34" s="3">
-        <v>0.98</v>
-      </c>
-      <c r="F34" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D35" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E35" s="3">
-        <v>0</v>
-      </c>
-      <c r="F35" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D36" s="1" t="s">
+      <c r="E38" s="3">
+        <v>0</v>
+      </c>
+      <c r="F38" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="G38" s="3">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="39" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="D39" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E39" s="3">
+        <v>0</v>
+      </c>
+      <c r="F39" s="3">
+        <v>0.72</v>
+      </c>
+      <c r="G39" s="3">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="40" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="D40" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E40" s="3">
+        <v>0</v>
+      </c>
+      <c r="F40" s="3">
+        <v>0.26</v>
+      </c>
+      <c r="G40" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="3:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D41" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E36" s="3">
-        <v>0.83</v>
-      </c>
-      <c r="F36" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D37" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E37" s="1">
-        <v>3.928356</v>
-      </c>
-      <c r="F37" s="1">
-        <v>51.211255000000001</v>
-      </c>
-    </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C38" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E38" s="3">
-        <v>0.35</v>
-      </c>
-      <c r="F38" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D39" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E39" s="3">
-        <v>0</v>
-      </c>
-      <c r="F39" s="3">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D40" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E40" s="3">
-        <v>0</v>
-      </c>
-      <c r="F40" s="3">
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D41" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="E41" s="3">
         <v>0</v>
       </c>
       <c r="F41" s="3">
-        <v>0.26</v>
-      </c>
-    </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="G41" s="3">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D42" s="1" t="s">
         <v>13</v>
       </c>
@@ -972,8 +1041,11 @@
       <c r="F42" s="1">
         <v>46.532781</v>
       </c>
-    </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="G42" s="6">
+        <v>46.448174999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C43" s="1" t="s">
         <v>7</v>
       </c>
@@ -986,8 +1058,11 @@
       <c r="F43" s="3">
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="44" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="G43" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D44" s="1" t="s">
         <v>13</v>
       </c>
@@ -996,6 +1071,9 @@
       </c>
       <c r="F44" s="1">
         <v>46.836553000000002</v>
+      </c>
+      <c r="G44" s="6">
+        <v>46.158969999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>